<commit_message>
data driver from xsel file
</commit_message>
<xml_diff>
--- a/craftBetAutomation/src/test/java/testData/InvalidData.xlsx
+++ b/craftBetAutomation/src/test/java/testData/InvalidData.xlsx
@@ -3,24 +3,35 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23478F5-FE78-4A99-9D70-F9069B1D26A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805F4408-8459-4AFA-B575-CBD5CF1C47B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1590" windowWidth="21600" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1590" windowWidth="21600" windowHeight="11355" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginInvalidData" sheetId="1" r:id="rId1"/>
+    <sheet name="PasswordRecoveryInvalidData" sheetId="2" r:id="rId2"/>
+    <sheet name="SignUpQuickInvalidEmail" sheetId="3" r:id="rId3"/>
+    <sheet name="SignUpQuickInvalidNumber" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>username</t>
   </si>
@@ -59,13 +70,58 @@
   </si>
   <si>
     <t>N3H U3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> g.babloyan@iqsoft.am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g.babloyan@iqsoft.am </t>
+  </si>
+  <si>
+    <t>g .babloyan@iqsoft.am</t>
+  </si>
+  <si>
+    <t>g. babloyan@iqsoft.am</t>
+  </si>
+  <si>
+    <t>g.babloyan@iqsoft.a m</t>
+  </si>
+  <si>
+    <t>0.12/34?56</t>
+  </si>
+  <si>
+    <t>123abc123</t>
+  </si>
+  <si>
+    <t>g_babloyan@mail.com</t>
+  </si>
+  <si>
+    <t>gor@babloyan@mail.ru</t>
+  </si>
+  <si>
+    <t>Email/Password</t>
+  </si>
+  <si>
+    <t>123 45 6</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>123/45/6</t>
+  </si>
+  <si>
+    <t>123+45-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 2 3 4 5 6 7 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +154,33 @@
       <sz val="9.8000000000000007"/>
       <color rgb="FFA9B7C6"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -138,18 +221,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -462,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -530,9 +636,208 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:2" ht="23.25">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="23.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="23.25">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B107D13E-A346-41E9-BA28-C19551100D77}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="47.5703125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="23.25">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="7">
+        <v>23456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="7">
+        <v>2345678900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="7">
+        <v>0.123456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1" xr:uid="{1F26CA27-A05C-4C46-B12D-5ADBBE613F47}"/>
+    <hyperlink ref="A9" r:id="rId2" xr:uid="{229E86E5-BEC2-441E-A258-A596E80E5D30}"/>
+    <hyperlink ref="A13" r:id="rId3" xr:uid="{B47E7718-FA6B-4774-862F-2B448051A7ED}"/>
+    <hyperlink ref="A14" r:id="rId4" xr:uid="{28318217-EAC3-40DA-8429-CEB3BEB90B75}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9F1D9D-D877-4A36-A600-C8C884B5C43A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B796E1-4559-41F4-9FB3-C3AB336F6B3F}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="23.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="7">
+        <v>23456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="5">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="5">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>